<commit_message>
added ad blocker extension
</commit_message>
<xml_diff>
--- a/code/database/data_extract.xlsx
+++ b/code/database/data_extract.xlsx
@@ -1,20 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fatim\Desktop\crawl\code\database\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="12" windowWidth="16092" windowHeight="9660"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -792,8 +787,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -852,14 +847,6 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -906,7 +893,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -938,10 +925,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -973,7 +959,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1149,24 +1134,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E84"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="40.77734375" customWidth="1"/>
-    <col min="2" max="2" width="8" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="41.33203125" customWidth="1"/>
-    <col min="4" max="4" width="14.109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="41.33203125" customWidth="1"/>
-    <col min="6" max="41" width="9.109375"/>
+    <col min="1" max="1" width="40.7109375" customWidth="1"/>
+    <col min="2" max="2" width="8.7109375" customWidth="1"/>
+    <col min="3" max="3" width="40.7109375" customWidth="1"/>
+    <col min="4" max="4" width="14.7109375" customWidth="1"/>
+    <col min="5" max="5" width="40.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1183,7 +1165,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5">
       <c r="A2" s="2" t="s">
         <v>5</v>
       </c>
@@ -1200,7 +1182,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5">
       <c r="A3" s="2" t="s">
         <v>9</v>
       </c>
@@ -1217,7 +1199,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5">
       <c r="A4" s="2" t="s">
         <v>12</v>
       </c>
@@ -1234,7 +1216,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5">
       <c r="A5" s="2" t="s">
         <v>15</v>
       </c>
@@ -1251,7 +1233,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5">
       <c r="A6" s="2" t="s">
         <v>18</v>
       </c>
@@ -1268,7 +1250,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5">
       <c r="A7" s="2" t="s">
         <v>21</v>
       </c>
@@ -1285,7 +1267,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5">
       <c r="A8" s="2" t="s">
         <v>24</v>
       </c>
@@ -1302,7 +1284,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5">
       <c r="A9" s="2" t="s">
         <v>27</v>
       </c>
@@ -1319,7 +1301,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5">
       <c r="A10" s="2" t="s">
         <v>30</v>
       </c>
@@ -1336,7 +1318,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5">
       <c r="A11" s="2" t="s">
         <v>33</v>
       </c>
@@ -1353,7 +1335,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5">
       <c r="A12" s="2" t="s">
         <v>36</v>
       </c>
@@ -1370,7 +1352,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5">
       <c r="A13" s="2" t="s">
         <v>39</v>
       </c>
@@ -1387,7 +1369,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5">
       <c r="A14" s="2" t="s">
         <v>42</v>
       </c>
@@ -1404,7 +1386,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5">
       <c r="A15" s="2" t="s">
         <v>45</v>
       </c>
@@ -1421,7 +1403,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5">
       <c r="A16" s="2" t="s">
         <v>48</v>
       </c>
@@ -1438,7 +1420,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5">
       <c r="A17" s="2" t="s">
         <v>51</v>
       </c>
@@ -1455,7 +1437,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5">
       <c r="A18" s="2" t="s">
         <v>54</v>
       </c>
@@ -1472,7 +1454,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5">
       <c r="A19" s="2" t="s">
         <v>57</v>
       </c>
@@ -1489,7 +1471,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:5">
       <c r="A20" s="2" t="s">
         <v>60</v>
       </c>
@@ -1506,7 +1488,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:5">
       <c r="A21" s="2" t="s">
         <v>63</v>
       </c>
@@ -1523,7 +1505,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:5">
       <c r="A22" s="2" t="s">
         <v>66</v>
       </c>
@@ -1540,7 +1522,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:5">
       <c r="A23" s="2" t="s">
         <v>69</v>
       </c>
@@ -1557,7 +1539,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:5">
       <c r="A24" s="2" t="s">
         <v>72</v>
       </c>
@@ -1574,7 +1556,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:5">
       <c r="A25" s="2" t="s">
         <v>75</v>
       </c>
@@ -1591,7 +1573,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:5">
       <c r="A26" s="2" t="s">
         <v>78</v>
       </c>
@@ -1608,7 +1590,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:5">
       <c r="A27" s="2" t="s">
         <v>81</v>
       </c>
@@ -1625,7 +1607,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:5">
       <c r="A28" s="2" t="s">
         <v>84</v>
       </c>
@@ -1642,7 +1624,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:5">
       <c r="A29" s="2" t="s">
         <v>87</v>
       </c>
@@ -1659,7 +1641,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:5">
       <c r="A30" s="2" t="s">
         <v>90</v>
       </c>
@@ -1676,7 +1658,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:5">
       <c r="A31" s="2" t="s">
         <v>93</v>
       </c>
@@ -1693,7 +1675,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:5">
       <c r="A32" s="2" t="s">
         <v>96</v>
       </c>
@@ -1710,7 +1692,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:5">
       <c r="A33" s="2" t="s">
         <v>100</v>
       </c>
@@ -1727,7 +1709,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:5">
       <c r="A34" s="2" t="s">
         <v>103</v>
       </c>
@@ -1744,7 +1726,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:5">
       <c r="A35" s="2" t="s">
         <v>106</v>
       </c>
@@ -1761,7 +1743,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:5">
       <c r="A36" s="2" t="s">
         <v>109</v>
       </c>
@@ -1778,7 +1760,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:5">
       <c r="A37" s="2" t="s">
         <v>112</v>
       </c>
@@ -1795,7 +1777,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:5">
       <c r="A38" s="2" t="s">
         <v>115</v>
       </c>
@@ -1812,7 +1794,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:5">
       <c r="A39" s="2" t="s">
         <v>118</v>
       </c>
@@ -1829,7 +1811,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:5">
       <c r="A40" s="2" t="s">
         <v>121</v>
       </c>
@@ -1846,7 +1828,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:5">
       <c r="A41" s="2" t="s">
         <v>124</v>
       </c>
@@ -1863,7 +1845,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:5">
       <c r="A42" s="2" t="s">
         <v>127</v>
       </c>
@@ -1880,7 +1862,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:5">
       <c r="A43" s="2" t="s">
         <v>130</v>
       </c>
@@ -1897,7 +1879,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:5">
       <c r="A44" s="2" t="s">
         <v>133</v>
       </c>
@@ -1914,7 +1896,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:5">
       <c r="A45" s="2" t="s">
         <v>136</v>
       </c>
@@ -1931,7 +1913,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:5">
       <c r="A46" s="2" t="s">
         <v>139</v>
       </c>
@@ -1948,7 +1930,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:5">
       <c r="A47" s="2" t="s">
         <v>142</v>
       </c>
@@ -1965,7 +1947,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:5">
       <c r="A48" s="2" t="s">
         <v>145</v>
       </c>
@@ -1982,7 +1964,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:5">
       <c r="A49" s="2" t="s">
         <v>148</v>
       </c>
@@ -1999,7 +1981,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:5">
       <c r="A50" s="2" t="s">
         <v>151</v>
       </c>
@@ -2016,7 +1998,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:5">
       <c r="A51" s="2" t="s">
         <v>154</v>
       </c>
@@ -2033,7 +2015,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:5">
       <c r="A52" s="2" t="s">
         <v>157</v>
       </c>
@@ -2050,7 +2032,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:5">
       <c r="A53" s="2" t="s">
         <v>160</v>
       </c>
@@ -2067,7 +2049,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:5">
       <c r="A54" s="2" t="s">
         <v>163</v>
       </c>
@@ -2084,7 +2066,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:5">
       <c r="A55" s="2" t="s">
         <v>166</v>
       </c>
@@ -2101,7 +2083,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:5">
       <c r="A56" s="2" t="s">
         <v>169</v>
       </c>
@@ -2118,7 +2100,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:5">
       <c r="A57" s="2" t="s">
         <v>172</v>
       </c>
@@ -2135,7 +2117,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:5">
       <c r="A58" s="2" t="s">
         <v>175</v>
       </c>
@@ -2152,7 +2134,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:5">
       <c r="A59" s="2" t="s">
         <v>178</v>
       </c>
@@ -2169,7 +2151,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:5">
       <c r="A60" s="2" t="s">
         <v>181</v>
       </c>
@@ -2186,7 +2168,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:5">
       <c r="A61" s="2" t="s">
         <v>184</v>
       </c>
@@ -2203,7 +2185,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:5">
       <c r="A62" s="2" t="s">
         <v>187</v>
       </c>
@@ -2220,7 +2202,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:5">
       <c r="A63" s="2" t="s">
         <v>190</v>
       </c>
@@ -2237,7 +2219,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:5">
       <c r="A64" s="2" t="s">
         <v>193</v>
       </c>
@@ -2254,7 +2236,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:5">
       <c r="A65" s="2" t="s">
         <v>196</v>
       </c>
@@ -2271,7 +2253,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:5">
       <c r="A66" s="2" t="s">
         <v>199</v>
       </c>
@@ -2288,7 +2270,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:5">
       <c r="A67" s="2" t="s">
         <v>202</v>
       </c>
@@ -2305,7 +2287,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:5">
       <c r="A68" s="2" t="s">
         <v>205</v>
       </c>
@@ -2322,7 +2304,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:5">
       <c r="A69" s="2" t="s">
         <v>208</v>
       </c>
@@ -2339,7 +2321,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:5">
       <c r="A70" s="2" t="s">
         <v>211</v>
       </c>
@@ -2356,7 +2338,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:5">
       <c r="A71" s="2" t="s">
         <v>214</v>
       </c>
@@ -2373,7 +2355,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:5">
       <c r="A72" s="2" t="s">
         <v>217</v>
       </c>
@@ -2390,7 +2372,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:5">
       <c r="A73" s="2" t="s">
         <v>220</v>
       </c>
@@ -2407,7 +2389,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:5">
       <c r="A74" s="2" t="s">
         <v>223</v>
       </c>
@@ -2424,7 +2406,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:5">
       <c r="A75" s="2" t="s">
         <v>226</v>
       </c>
@@ -2441,7 +2423,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:5">
       <c r="A76" s="2" t="s">
         <v>229</v>
       </c>
@@ -2458,7 +2440,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:5">
       <c r="A77" s="2" t="s">
         <v>232</v>
       </c>
@@ -2475,7 +2457,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:5">
       <c r="A78" s="2" t="s">
         <v>235</v>
       </c>
@@ -2492,7 +2474,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:5">
       <c r="A79" s="2" t="s">
         <v>238</v>
       </c>
@@ -2509,7 +2491,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:5">
       <c r="A80" s="2" t="s">
         <v>241</v>
       </c>
@@ -2526,7 +2508,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:5">
       <c r="A81" s="2" t="s">
         <v>244</v>
       </c>
@@ -2543,7 +2525,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:5">
       <c r="A82" s="2" t="s">
         <v>247</v>
       </c>
@@ -2560,7 +2542,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:5">
       <c r="A83" s="2" t="s">
         <v>250</v>
       </c>
@@ -2577,7 +2559,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:5">
       <c r="A84" s="2" t="s">
         <v>253</v>
       </c>

</xml_diff>